<commit_message>
Receita batendo, impostos ainda não
</commit_message>
<xml_diff>
--- a/Atividades_Duke_v2.xlsx
+++ b/Atividades_Duke_v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Dropbox\Corporate Office\Duke_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Documents\GitHub\Duke\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="19200" windowHeight="11580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>IR diferido</t>
   </si>
@@ -240,15 +240,9 @@
     <t>Pedir entradas TJLP e CDI</t>
   </si>
   <si>
-    <t>Cobrar planilha de debêntures</t>
-  </si>
-  <si>
     <t>Sobre os dados de contrato (Fábio) - só Forecast mesmo?</t>
   </si>
   <si>
-    <t>esqueleto de saida balanço</t>
-  </si>
-  <si>
     <t>Amortização a menos de 30 dias</t>
   </si>
   <si>
@@ -262,6 +256,21 @@
   </si>
   <si>
     <t>Finalizar, atualizar param_struct</t>
+  </si>
+  <si>
+    <t>Fabio:</t>
+  </si>
+  <si>
+    <t>Apenas Paranapanema</t>
+  </si>
+  <si>
+    <t>Incluir coluna de Agreement_type</t>
+  </si>
+  <si>
+    <t>Perguntar sobre o tax_rate dos contratos</t>
+  </si>
+  <si>
+    <t>Como funciona o inflacionamento dos contratos?</t>
   </si>
 </sst>
 </file>
@@ -634,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G44"/>
+  <dimension ref="B2:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,10 +1088,10 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D29" s="4">
         <v>2</v>
@@ -1096,10 +1105,10 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="4">
         <v>4</v>
@@ -1145,7 +1154,7 @@
         <v>63</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
@@ -1179,7 +1188,7 @@
         <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
@@ -1208,7 +1217,7 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
@@ -1221,14 +1230,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>73</v>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>